<commit_message>
Bring up to v0.27.3
</commit_message>
<xml_diff>
--- a/Documentation/Slots.xlsx
+++ b/Documentation/Slots.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="21075" windowHeight="9525"/>
+    <workbookView xWindow="120" yWindow="105" windowWidth="21075" windowHeight="9525" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="TROOP" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5105" uniqueCount="1191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5135" uniqueCount="1206">
   <si>
     <t>Native</t>
   </si>
@@ -3672,6 +3672,51 @@
   </si>
   <si>
     <t>Tracks that a name has already been altered.</t>
+  </si>
+  <si>
+    <t>slot_troop_in_player_merc_group</t>
+  </si>
+  <si>
+    <t>Oathbound</t>
+  </si>
+  <si>
+    <t>Tracks if a companion was part of the player party prior to entering a contract or joining their party.</t>
+  </si>
+  <si>
+    <t>slot_faction_oathbound_rank</t>
+  </si>
+  <si>
+    <t>Represents your current rank within a faction.</t>
+  </si>
+  <si>
+    <t>slot_faction_oathbound_rating</t>
+  </si>
+  <si>
+    <t>Represents your current rating that sets your rank.</t>
+  </si>
+  <si>
+    <t>slot_faction_oathbound_reputation</t>
+  </si>
+  <si>
+    <t>Tracks how a trustworthy a faction feels you are.</t>
+  </si>
+  <si>
+    <t>slot_faction_oathbound_betrayals</t>
+  </si>
+  <si>
+    <t>Tracks how many times you've betrayed this faction.</t>
+  </si>
+  <si>
+    <t>slot_faction_oathbound_renewals</t>
+  </si>
+  <si>
+    <t>Tracks how many times you've renewed your contract with this faction.</t>
+  </si>
+  <si>
+    <t>slot_faction_oathbound_high_rank</t>
+  </si>
+  <si>
+    <t>Tracks the highest rank you've achieved with this faction to prevent emblem exploits.</t>
   </si>
 </sst>
 </file>
@@ -4355,11 +4400,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L742"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B143" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="85" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="C143" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C160" sqref="C160"/>
+      <selection pane="bottomRight" activeCell="C162" sqref="C162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7238,19 +7283,31 @@
         <v>818</v>
       </c>
     </row>
-    <row r="161" spans="1:12">
+    <row r="161" spans="1:12" ht="30">
       <c r="A161" s="4">
         <v>159</v>
       </c>
-      <c r="C161" s="32"/>
-      <c r="D161" s="32"/>
-      <c r="E161" s="33"/>
-      <c r="F161" s="34"/>
-      <c r="G161" s="35"/>
+      <c r="C161" s="32" t="s">
+        <v>1191</v>
+      </c>
+      <c r="D161" s="32" t="s">
+        <v>1192</v>
+      </c>
+      <c r="E161" s="33" t="s">
+        <v>1193</v>
+      </c>
+      <c r="F161" s="34" t="s">
+        <v>977</v>
+      </c>
+      <c r="G161" s="35" t="s">
+        <v>602</v>
+      </c>
       <c r="H161" s="34"/>
       <c r="I161" s="34"/>
       <c r="J161" s="34"/>
-      <c r="K161" s="34"/>
+      <c r="K161" s="34" t="s">
+        <v>818</v>
+      </c>
       <c r="L161" s="34"/>
     </row>
     <row r="162" spans="1:12">
@@ -32999,11 +33056,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H742"/>
   <sheetViews>
-    <sheetView zoomScale="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B275" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C12" sqref="C12"/>
+      <selection pane="bottomRight" activeCell="G287" sqref="G287"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -36004,82 +36061,172 @@
         <v>270</v>
       </c>
     </row>
-    <row r="273" spans="1:1">
+    <row r="273" spans="1:7">
       <c r="A273" s="4">
         <v>271</v>
       </c>
     </row>
-    <row r="274" spans="1:1">
+    <row r="274" spans="1:7">
       <c r="A274" s="4">
         <v>272</v>
       </c>
     </row>
-    <row r="275" spans="1:1">
+    <row r="275" spans="1:7">
       <c r="A275" s="4">
         <v>273</v>
       </c>
     </row>
-    <row r="276" spans="1:1">
+    <row r="276" spans="1:7">
       <c r="A276" s="4">
         <v>274</v>
       </c>
     </row>
-    <row r="277" spans="1:1">
+    <row r="277" spans="1:7">
       <c r="A277" s="4">
         <v>275</v>
       </c>
     </row>
-    <row r="278" spans="1:1">
+    <row r="278" spans="1:7">
       <c r="A278" s="4">
         <v>276</v>
       </c>
     </row>
-    <row r="279" spans="1:1">
+    <row r="279" spans="1:7">
       <c r="A279" s="4">
         <v>277</v>
       </c>
     </row>
-    <row r="280" spans="1:1">
+    <row r="280" spans="1:7">
       <c r="A280" s="4">
         <v>278</v>
       </c>
     </row>
-    <row r="281" spans="1:1">
+    <row r="281" spans="1:7">
       <c r="A281" s="4">
         <v>279</v>
       </c>
     </row>
-    <row r="282" spans="1:1">
+    <row r="282" spans="1:7">
       <c r="A282" s="4">
         <v>280</v>
       </c>
-    </row>
-    <row r="283" spans="1:1">
+      <c r="C282" s="6" t="s">
+        <v>1194</v>
+      </c>
+      <c r="D282" s="6" t="s">
+        <v>1192</v>
+      </c>
+      <c r="E282" s="3" t="s">
+        <v>1195</v>
+      </c>
+      <c r="F282">
+        <v>0</v>
+      </c>
+      <c r="G282" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="283" spans="1:7">
       <c r="A283" s="4">
         <v>281</v>
       </c>
-    </row>
-    <row r="284" spans="1:1">
+      <c r="C283" s="6" t="s">
+        <v>1196</v>
+      </c>
+      <c r="D283" s="6" t="s">
+        <v>1192</v>
+      </c>
+      <c r="E283" s="3" t="s">
+        <v>1197</v>
+      </c>
+      <c r="F283">
+        <v>0</v>
+      </c>
+      <c r="G283" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="284" spans="1:7">
       <c r="A284" s="4">
         <v>282</v>
       </c>
-    </row>
-    <row r="285" spans="1:1">
+      <c r="C284" s="6" t="s">
+        <v>1198</v>
+      </c>
+      <c r="D284" s="6" t="s">
+        <v>1192</v>
+      </c>
+      <c r="E284" s="3" t="s">
+        <v>1199</v>
+      </c>
+      <c r="F284">
+        <v>0</v>
+      </c>
+      <c r="G284" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="285" spans="1:7">
       <c r="A285" s="4">
         <v>283</v>
       </c>
-    </row>
-    <row r="286" spans="1:1">
+      <c r="C285" s="6" t="s">
+        <v>1200</v>
+      </c>
+      <c r="D285" s="6" t="s">
+        <v>1192</v>
+      </c>
+      <c r="E285" s="3" t="s">
+        <v>1201</v>
+      </c>
+      <c r="F285">
+        <v>0</v>
+      </c>
+      <c r="G285" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="286" spans="1:7" ht="30">
       <c r="A286" s="4">
         <v>284</v>
       </c>
-    </row>
-    <row r="287" spans="1:1">
+      <c r="C286" s="6" t="s">
+        <v>1202</v>
+      </c>
+      <c r="D286" s="6" t="s">
+        <v>1192</v>
+      </c>
+      <c r="E286" s="3" t="s">
+        <v>1203</v>
+      </c>
+      <c r="F286">
+        <v>0</v>
+      </c>
+      <c r="G286" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="287" spans="1:7" ht="30">
       <c r="A287" s="4">
         <v>285</v>
       </c>
-    </row>
-    <row r="288" spans="1:1">
+      <c r="C287" s="6" t="s">
+        <v>1204</v>
+      </c>
+      <c r="D287" s="6" t="s">
+        <v>1192</v>
+      </c>
+      <c r="E287" s="3" t="s">
+        <v>1205</v>
+      </c>
+      <c r="F287">
+        <v>0</v>
+      </c>
+      <c r="G287" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="288" spans="1:7">
       <c r="A288" s="4">
         <v>286</v>
       </c>

</xml_diff>